<commit_message>
Updated Vols golf original data.
</commit_message>
<xml_diff>
--- a/mengolf/original_data/mengolf.xlsx
+++ b/mengolf/original_data/mengolf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/User/student/Documents/GitHub/athletics/mengolf/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436C1250-C0E8-594A-8D11-160C70E86317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EF795C-65DA-F342-931B-37A81115F333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,9 +235,6 @@
     <t>Tennessee 1997-98 golf guide</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 1997-1998</t>
-  </si>
-  <si>
     <t>1997</t>
   </si>
   <si>
@@ -248,9 +245,6 @@
   </si>
   <si>
     <t>1998-99 men's golf guide: Tennessee</t>
-  </si>
-  <si>
-    <t>University of Tennessee Volunteers, golf media guide 1998-1999</t>
   </si>
   <si>
     <t>1998</t>
@@ -268,9 +262,6 @@
     <t>1999-2000 men's golf: Tennessee</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 1999-2000</t>
-  </si>
-  <si>
     <t>1999</t>
   </si>
   <si>
@@ -283,9 +274,6 @@
     <t>Tennessee 2001 men's golf</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 2000-2001</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
@@ -293,9 +281,6 @@
   </si>
   <si>
     <t>Tennessee 2002 men's golf</t>
-  </si>
-  <si>
-    <t>University of Tennessee Volunteers, golf media guide 2001-2002</t>
   </si>
   <si>
     <t>2001</t>
@@ -310,9 +295,6 @@
     <t>2002-03 University of Tennessee Volunteers golf guide</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 2002-2003</t>
-  </si>
-  <si>
     <t>2002</t>
   </si>
   <si>
@@ -320,9 +302,6 @@
   </si>
   <si>
     <t>Tennessee 2003-04 men's golf</t>
-  </si>
-  <si>
-    <t>University of Tennessee Volunteers, golf media guide 2003-2004</t>
   </si>
   <si>
     <t>2003</t>
@@ -337,9 +316,6 @@
     <t>2004-05 Volunteer golf: major intentions</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 2004-2005</t>
-  </si>
-  <si>
     <t>2004</t>
   </si>
   <si>
@@ -352,25 +328,16 @@
     <t>2005-06 Volunteers golf</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 2005-2006</t>
-  </si>
-  <si>
     <t>2005</t>
   </si>
   <si>
     <t>2006-07 Volunteer golf</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 2006-2007</t>
-  </si>
-  <si>
     <t>2006</t>
   </si>
   <si>
     <t>2007-08 Volunteers golf</t>
-  </si>
-  <si>
-    <t>University of Tennessee Volunteers, golf media guide 2007-2008</t>
   </si>
   <si>
     <t>2007</t>
@@ -382,9 +349,6 @@
     <t>2008-09 Volunteers golf</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 2008-2009</t>
-  </si>
-  <si>
     <t>2008</t>
   </si>
   <si>
@@ -394,9 +358,6 @@
     <t>Volunteers Tennessee 2009-10 golf</t>
   </si>
   <si>
-    <t>University of Tennessee Volunteers, golf media guide 2009-2010</t>
-  </si>
-  <si>
     <t>2009</t>
   </si>
   <si>
@@ -404,6 +365,45 @@
   </si>
   <si>
     <t>booklet</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 1997-1998</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 1998-1999</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 1999-2000</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2001-2002</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2000-2001</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2002-2003</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2003-2004</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2004-2005</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2005-2006</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2006-2007</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2007-2008</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2008-2009</t>
+  </si>
+  <si>
+    <t>University of Tennessee Volunteers golf media guide, 2009-2010</t>
   </si>
 </sst>
 </file>
@@ -760,7 +760,7 @@
   <dimension ref="A1:U958"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1322,16 +1322,16 @@
         <v>67</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>43</v>
@@ -1382,22 +1382,22 @@
         <v>vols-golf_1998</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="D10" s="9" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>43</v>
@@ -1418,7 +1418,7 @@
         <v>37</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>25</v>
@@ -1448,22 +1448,22 @@
         <v>vols-golf_1999</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>43</v>
@@ -1484,7 +1484,7 @@
         <v>37</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>25</v>
@@ -1514,22 +1514,22 @@
         <v>vols-golf_2000</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>43</v>
@@ -1550,7 +1550,7 @@
         <v>37</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>25</v>
@@ -1580,22 +1580,22 @@
         <v>vols-golf_2001</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>43</v>
@@ -1616,7 +1616,7 @@
         <v>37</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>25</v>
@@ -1646,22 +1646,22 @@
         <v>vols-golf_2002</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>43</v>
@@ -1682,7 +1682,7 @@
         <v>37</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O14" s="7" t="s">
         <v>25</v>
@@ -1712,22 +1712,22 @@
         <v>vols-golf_2003</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>43</v>
@@ -1748,7 +1748,7 @@
         <v>37</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>25</v>
@@ -1778,22 +1778,22 @@
         <v>vols-golf_2004</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>43</v>
@@ -1814,7 +1814,7 @@
         <v>37</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>25</v>
@@ -1844,22 +1844,22 @@
         <v>vols-golf_2005</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>43</v>
@@ -1880,7 +1880,7 @@
         <v>37</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O17" s="7" t="s">
         <v>25</v>
@@ -1910,22 +1910,22 @@
         <v>vols-golf_2006</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>43</v>
@@ -1946,7 +1946,7 @@
         <v>37</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O18" s="7" t="s">
         <v>25</v>
@@ -1976,22 +1976,22 @@
         <v>vols-golf_2007</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>43</v>
@@ -2012,7 +2012,7 @@
         <v>37</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O19" s="7" t="s">
         <v>25</v>
@@ -2036,28 +2036,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="71" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"vols-golf_2008")</f>
         <v>vols-golf_2008</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>43</v>
@@ -2078,7 +2078,7 @@
         <v>37</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O20" s="7" t="s">
         <v>25</v>
@@ -2102,26 +2102,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="71" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"vols-golf_2009")</f>
         <v>vols-golf_2009</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="9" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>43</v>
@@ -2142,7 +2142,7 @@
         <v>37</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O21" s="7" t="s">
         <v>25</v>
@@ -2154,7 +2154,7 @@
         <v>27</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="S21" s="9" t="s">
         <v>29</v>

</xml_diff>